<commit_message>
added images and tables, experiment 1-4
</commit_message>
<xml_diff>
--- a/code/results/experiment1/Experiment1-Table.xlsx
+++ b/code/results/experiment1/Experiment1-Table.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maarten\Desktop\Afstuderen\thesis_stock_prediction_repo\code\results\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E901A76-4D8A-416D-9E9C-E736C7BA798E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C47CE0-BC07-4FE9-9210-5350B8A3A2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment1-Table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,9 +54,6 @@
     <t>MSFT</t>
   </si>
   <si>
-    <t>5_imputations_combined</t>
-  </si>
-  <si>
     <t>cubicfit260</t>
   </si>
   <si>
@@ -59,12 +67,18 @@
   </si>
   <si>
     <t>meanlast260</t>
+  </si>
+  <si>
+    <t>5 imputations combined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -125,6 +139,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +484,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,232 +501,232 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.593715636511822E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.619540958382014E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>2.593715636511822E-2</v>
-      </c>
-      <c r="D2">
-        <v>1.619540958382014E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="4">
+        <v>4.1027874288724717E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.259056326408963E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>4.1027874288724717E-2</v>
-      </c>
-      <c r="D3">
-        <v>3.259056326408963E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="4">
+        <v>2.8975586177759641E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.236836671755697E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>2.8975586177759641E-2</v>
-      </c>
-      <c r="D4">
-        <v>3.236836671755697E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="4">
+        <v>3.3550456152901052E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.46613702749347E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>3.3550456152901052E-2</v>
-      </c>
-      <c r="D5">
-        <v>3.46613702749347E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="4">
+        <v>2.9873173936255819E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.0300335614928809E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>2.9873173936255819E-2</v>
-      </c>
-      <c r="D6">
-        <v>2.0300335614928809E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="4">
+        <v>2.829020347151218E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.505415027126685E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>2.829020347151218E-2</v>
-      </c>
-      <c r="D7">
-        <v>1.505415027126685E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="4">
+        <v>1.432684145126336E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.661560690676939E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>1.432684145126336E-2</v>
-      </c>
-      <c r="D8">
-        <v>1.661560690676939E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="4">
+        <v>9.1962179706676275E-3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3.8104049476411308E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>9.1962179706676275E-3</v>
-      </c>
-      <c r="D9">
-        <v>3.8104049476411308E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="4">
+        <v>6.2569445630792277E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.4570415472449148E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>6.2569445630792277E-3</v>
-      </c>
-      <c r="D10">
-        <v>2.4570415472449148E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="4">
+        <v>1.155010249216405E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.029678271726648E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>1.155010249216405E-2</v>
-      </c>
-      <c r="D11">
-        <v>1.029678271726648E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="4">
+        <v>1.1234121630536701E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.7937265985414906E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>1.1234121630536701E-2</v>
-      </c>
-      <c r="D12">
-        <v>8.7937265985414906E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="4">
+        <v>1.2073951173137981E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.2613786442686041E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>1.2073951173137981E-2</v>
-      </c>
-      <c r="D13">
-        <v>1.2613786442686041E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="4">
+        <v>1.9426464964520981E-2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.0125308471514638E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14">
-        <v>1.9426464964520981E-2</v>
-      </c>
-      <c r="D14">
-        <v>2.0125308471514638E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="4">
+        <v>2.20656177707792E-2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.7123943483010259E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15">
-        <v>2.20656177707792E-2</v>
-      </c>
-      <c r="D15">
-        <v>1.7123943483010259E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="4">
+        <v>3.0076075222619739E-2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.305709553748346E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16">
-        <v>3.0076075222619739E-2</v>
-      </c>
-      <c r="D16">
-        <v>2.305709553748346E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="4">
+        <v>1.9096669762790421E-2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.9886378300791731E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17">
-        <v>1.9096669762790421E-2</v>
-      </c>
-      <c r="D17">
-        <v>3.9886378300791731E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="4">
+        <v>2.2115173050738578E-2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3.5628856741183048E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18">
-        <v>2.2115173050738578E-2</v>
-      </c>
-      <c r="D18">
-        <v>3.5628856741183048E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>2.6560691811598602E-2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>1.553396089326717E-2</v>
       </c>
     </row>

</xml_diff>